<commit_message>
update the backend 4/16/2025
</commit_message>
<xml_diff>
--- a/static/students.xlsx
+++ b/static/students.xlsx
@@ -791,17 +791,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>email0@gmail.com</t>
+          <t>email5@gmail.com</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>School0</t>
+          <t>School5</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -811,32 +811,32 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Battambang</t>
+          <t>Siem Reap</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>23123</t>
+          <t>57906</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>15/04/2025</t>
+          <t>16/04/2025</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>21:57:14</t>
+          <t>21:32:07</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>B617</t>
+          <t>B330</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>School0</t>
+          <t>School5</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">

</xml_diff>

<commit_message>
Add Table Image 4/22/2025 at ngiht time 10:57
</commit_message>
<xml_diff>
--- a/static/students.xlsx
+++ b/static/students.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,30 +464,35 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>Image Filename</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>SEL</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Tran Date</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Code</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Loc</t>
         </is>
@@ -501,11 +506,13 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Surname0</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>21</v>
+          <t>Username0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -529,35 +536,40 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Siem Reap</t>
+          <t>Battambang</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>92590</t>
+          <t>Name0_Username0_20250422_225605.jpg</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>10/04/2025</t>
+          <t>81991</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>21:08:41</t>
+          <t>22/04/2025</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>B238</t>
+          <t>22:56:05</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
+          <t>B821</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
           <t>School0</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>P</t>
         </is>
@@ -571,15 +583,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Surname1</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>22</v>
+          <t>UserName1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -604,242 +618,35 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>78134</t>
+          <t>Name1_UserName1_20250422_225703.png</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>10/04/2025</t>
+          <t>43575</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>21:09:28</t>
+          <t>22/04/2025</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>B710</t>
+          <t>22:57:03</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
+          <t>B944</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
           <t>School1</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Name3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Surname3</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>22</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>email3@gmail.com</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>School3</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>St 99 Hm20</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Phnom Penh</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>57156</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>10/04/2025</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>21:17:35</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>B124</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>School3</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Name4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Surname4</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>22</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>email4@gmail.com</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>School4</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>St 99 Hm20</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Phnom Penh</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>68762</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>10/04/2025</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>21:17:54</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>B249</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>School4</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Name5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Username5</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>email5@gmail.com</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>School5</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>St 99 Hm20</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Siem Reap</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>57906</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>16/04/2025</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>21:32:07</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>B330</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>School5</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>P</t>
         </is>

</xml_diff>

<commit_message>
update the last 6/19/2025
</commit_message>
<xml_diff>
--- a/static/students.xlsx
+++ b/static/students.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -651,12 +651,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Name2</t>
+          <t>Name3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Username2</t>
+          <t>Username3</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -669,12 +669,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>email2@gmail.com</t>
+          <t>email3@gmail.com</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>School2</t>
+          <t>School3</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -684,117 +684,40 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Battambang</t>
+          <t>Siem Reap</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>image.jpg</t>
+          <t>dom.jpg</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>50385</t>
+          <t>25605</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>03/05/2025</t>
+          <t>11/05/2025</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>15:43:22</t>
+          <t>21:22:22</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>B162</t>
+          <t>B402</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>School2</t>
+          <t>School3</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Name3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Username3</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>email3@gmail.com</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>School3</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>St 99 Hm20</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Siem Reap</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>dom.jpg</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>25605</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>11/05/2025</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>21:22:22</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>B402</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>School3</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
         <is>
           <t>P</t>
         </is>

</xml_diff>